<commit_message>
Added latest changes on April 1st.
</commit_message>
<xml_diff>
--- a/FreeCRMTest/src/main/java/com/crm/qa/testdata/crm_new_company.xlsx
+++ b/FreeCRMTest/src/main/java/com/crm/qa/testdata/crm_new_company.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="2790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="2175"/>
   </bookViews>
   <sheets>
     <sheet name="new_company_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Company_Name</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>Employees</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>GT152</t>
+  </si>
+  <si>
+    <t>taxnum</t>
+  </si>
+  <si>
+    <t>phonenum</t>
+  </si>
+  <si>
+    <t>faxnum</t>
   </si>
 </sst>
 </file>
@@ -369,16 +384,20 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -394,6 +413,18 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -408,8 +439,19 @@
       <c r="D2">
         <v>1006</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>15422</v>
+      </c>
+      <c r="G2">
+        <v>112455</v>
+      </c>
+      <c r="H2">
+        <v>1548754</v>
+      </c>
+      <c r="I2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>